<commit_message>
Update data Lake Murten
</commit_message>
<xml_diff>
--- a/Data/LakeMurten/TP.xlsx
+++ b/Data/LakeMurten/TP.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Backup_Tomy\Data\Phosphorus\Model\phosphorus_model\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unils-my.sharepoint.com/personal/tomy_doda_unil_ch/Documents/External drive/Data/Phosphorus/Model/phosphorus_model/Data/LakeMurten/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_16E767CD8D0CE825C0645289CB49694582755D6E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -76,7 +77,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -90,13 +91,10 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3 3" xfId="1"/>
+    <cellStyle name="Normal 3 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -373,11 +371,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -557,124 +555,124 @@
       <c r="B8" s="4"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="F9" s="5"/>
+      <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
-      <c r="F10" s="5"/>
+      <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
-      <c r="F11" s="5"/>
+      <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
-      <c r="D12" s="5"/>
-      <c r="F12" s="5"/>
+      <c r="D12" s="4"/>
+      <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
-      <c r="D13" s="5"/>
-      <c r="F13" s="5"/>
+      <c r="D13" s="4"/>
+      <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
-      <c r="D14" s="5"/>
+      <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="D15" s="5"/>
-      <c r="F15" s="5"/>
+      <c r="D15" s="4"/>
+      <c r="F15" s="4"/>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
-      <c r="D16" s="5"/>
-      <c r="F16" s="5"/>
+      <c r="D16" s="4"/>
+      <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
-      <c r="D17" s="5"/>
-      <c r="F17" s="5"/>
+      <c r="D17" s="4"/>
+      <c r="F17" s="4"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
-      <c r="D18" s="5"/>
-      <c r="F18" s="5"/>
+      <c r="D18" s="4"/>
+      <c r="F18" s="4"/>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
-      <c r="D19" s="5"/>
-      <c r="F19" s="5"/>
+      <c r="D19" s="4"/>
+      <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
-      <c r="D20" s="5"/>
+      <c r="D20" s="4"/>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
-      <c r="D21" s="5"/>
-      <c r="F21" s="5"/>
+      <c r="D21" s="4"/>
+      <c r="F21" s="4"/>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
-      <c r="D22" s="5"/>
-      <c r="F22" s="5"/>
+      <c r="D22" s="4"/>
+      <c r="F22" s="4"/>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
-      <c r="D23" s="5"/>
-      <c r="F23" s="5"/>
+      <c r="D23" s="4"/>
+      <c r="F23" s="4"/>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
-      <c r="D24" s="5"/>
-      <c r="F24" s="5"/>
+      <c r="D24" s="4"/>
+      <c r="F24" s="4"/>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
-      <c r="D25" s="5"/>
-      <c r="F25" s="5"/>
+      <c r="D25" s="4"/>
+      <c r="F25" s="4"/>
     </row>
     <row r="26" spans="1:6">
-      <c r="D26" s="5"/>
+      <c r="D26" s="4"/>
     </row>
     <row r="27" spans="1:6">
-      <c r="D27" s="5"/>
+      <c r="D27" s="4"/>
     </row>
     <row r="28" spans="1:6">
-      <c r="D28" s="5"/>
+      <c r="D28" s="4"/>
     </row>
     <row r="29" spans="1:6">
-      <c r="D29" s="5"/>
+      <c r="D29" s="4"/>
     </row>
     <row r="30" spans="1:6">
-      <c r="D30" s="5"/>
+      <c r="D30" s="4"/>
     </row>
     <row r="31" spans="1:6">
-      <c r="D31" s="5"/>
+      <c r="D31" s="4"/>
     </row>
     <row r="32" spans="1:6">
-      <c r="D32" s="5"/>
+      <c r="D32" s="4"/>
     </row>
     <row r="33" spans="4:4">
-      <c r="D33" s="5"/>
+      <c r="D33" s="4"/>
     </row>
     <row r="34" spans="4:4">
-      <c r="D34" s="5"/>
+      <c r="D34" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>